<commit_message>
updated to 131 letters
</commit_message>
<xml_diff>
--- a/PH2017Mar23.xlsx
+++ b/PH2017Mar23.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="860" yWindow="520" windowWidth="23340" windowHeight="14500"/>
+    <workbookView xWindow="840" yWindow="460" windowWidth="27960" windowHeight="17540"/>
   </bookViews>
   <sheets>
     <sheet name="Attendees" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2727" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2869" uniqueCount="387">
   <si>
     <t>Order #</t>
   </si>
@@ -1130,25 +1130,64 @@
     <t>mlkimmel@comcast.net</t>
   </si>
   <si>
-    <t>Infections in IBD</t>
-  </si>
-  <si>
-    <t>Experience of IBD Surgery</t>
-  </si>
-  <si>
-    <t>session1</t>
-  </si>
-  <si>
-    <t>session2</t>
-  </si>
-  <si>
-    <t>session3</t>
-  </si>
-  <si>
-    <t>session4</t>
-  </si>
-  <si>
-    <t>session5</t>
+    <t>Brittany</t>
+  </si>
+  <si>
+    <t>Schuler</t>
+  </si>
+  <si>
+    <t>brschuler@gmail.com</t>
+  </si>
+  <si>
+    <t>Heather</t>
+  </si>
+  <si>
+    <t>Polk</t>
+  </si>
+  <si>
+    <t>heather.polk@ucb.com</t>
+  </si>
+  <si>
+    <t>Austin</t>
+  </si>
+  <si>
+    <t>austin.r.maddox@gmail.com</t>
+  </si>
+  <si>
+    <t>Lynch</t>
+  </si>
+  <si>
+    <t>lynchem2@msu.edu</t>
+  </si>
+  <si>
+    <t>Gregory</t>
+  </si>
+  <si>
+    <t>Monahan</t>
+  </si>
+  <si>
+    <t>gregmonahanpbp@gmail.com</t>
+  </si>
+  <si>
+    <t>Corey</t>
+  </si>
+  <si>
+    <t>Hattaway</t>
+  </si>
+  <si>
+    <t>Coreyhattaway@gmail.com</t>
+  </si>
+  <si>
+    <t>Wigent</t>
+  </si>
+  <si>
+    <t>wigentk@yahoo.com</t>
+  </si>
+  <si>
+    <t>Kenniburg</t>
+  </si>
+  <si>
+    <t>kenniburgjohn@yahoo.com</t>
   </si>
 </sst>
 </file>
@@ -1158,18 +1197,13 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color rgb="FF000000"/>
-      <name val="Lucida Sans"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1192,10 +1226,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1497,22 +1530,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO123"/>
+  <dimension ref="A1:AG132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="96" workbookViewId="0">
-      <selection activeCell="Y9" sqref="A9:XFD9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="37" max="37" width="44.1640625" customWidth="1"/>
-    <col min="38" max="38" width="39.83203125" customWidth="1"/>
-    <col min="39" max="39" width="29.83203125" customWidth="1"/>
-    <col min="40" max="40" width="22" customWidth="1"/>
-    <col min="41" max="41" width="29" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1612,23 +1636,8 @@
       <c r="AG1" t="s">
         <v>32</v>
       </c>
-      <c r="AK1" t="s">
-        <v>369</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>370</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>371</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>372</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>373</v>
-      </c>
     </row>
-    <row r="2" spans="1:41" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>586466656</v>
       </c>
@@ -1692,58 +1701,8 @@
       <c r="V2" t="s">
         <v>40</v>
       </c>
-      <c r="W2" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="AA2" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="AC2" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="AF2" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>151</v>
-      </c>
-      <c r="AK2" t="str">
-        <f>W2</f>
-        <v>Will My Baby Develop IBD?</v>
-      </c>
-      <c r="AL2" t="str">
-        <f>X2</f>
-        <v>My Experience in Clinical Trials</v>
-      </c>
-      <c r="AM2" t="str">
-        <f>W3</f>
-        <v>What is IBD Remission: Adapting to a New Normal?</v>
-      </c>
-      <c r="AN2" t="str">
-        <f>AG2</f>
-        <v>Other or prefer not to say</v>
-      </c>
-      <c r="AO2" t="str">
-        <f>AD2</f>
-        <v>Acceptance in IBD &amp; Chronic Disease</v>
-      </c>
     </row>
-    <row r="3" spans="1:41" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>595209829</v>
       </c>
@@ -1810,55 +1769,8 @@
       <c r="W3" t="s">
         <v>44</v>
       </c>
-      <c r="X3" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="Y3" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AA3" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AB3" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="AC3" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="AD3" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AE3" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="AF3" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>151</v>
-      </c>
-      <c r="AK3" t="str">
-        <f>X3</f>
-        <v>Will My Baby Develop IBD?</v>
-      </c>
-      <c r="AL3" t="str">
-        <f>Y3</f>
-        <v>My Experience in Clinical Trials</v>
-      </c>
-      <c r="AM3" t="str">
-        <f>W3</f>
-        <v>What is IBD Remission: Adapting to a New Normal?</v>
-      </c>
-      <c r="AN3" t="str">
-        <f t="shared" ref="AN3:AN66" si="0">AG3</f>
-        <v>Other or prefer not to say</v>
-      </c>
-      <c r="AO3" t="str">
-        <f>AC3</f>
-        <v>Physical Therapy for Pain in IBD</v>
-      </c>
     </row>
-    <row r="4" spans="1:41" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>595209829</v>
       </c>
@@ -1925,55 +1837,8 @@
       <c r="W4" t="s">
         <v>48</v>
       </c>
-      <c r="X4" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="Y4" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AA4" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AB4" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="AC4" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="AD4" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AE4" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="AF4" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AG4" t="s">
-        <v>151</v>
-      </c>
-      <c r="AK4" t="str">
-        <f t="shared" ref="AK3:AK66" si="1">W4</f>
-        <v>Low FODMAP Diet in IBD</v>
-      </c>
-      <c r="AL4" t="str">
-        <f t="shared" ref="AL3:AL66" si="2">X4</f>
-        <v>Will My Baby Develop IBD?</v>
-      </c>
-      <c r="AM4" t="str">
-        <f>AF5</f>
-        <v>Parenting with IBD</v>
-      </c>
-      <c r="AN4" t="str">
-        <f t="shared" si="0"/>
-        <v>Other or prefer not to say</v>
-      </c>
-      <c r="AO4" t="str">
-        <f>AD2</f>
-        <v>Acceptance in IBD &amp; Chronic Disease</v>
-      </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>595232847</v>
       </c>
@@ -2067,30 +1932,8 @@
       <c r="AF5" t="s">
         <v>60</v>
       </c>
-      <c r="AG5" t="s">
-        <v>151</v>
-      </c>
-      <c r="AK5" t="str">
-        <f>X5</f>
-        <v>Antibiotics and Probiotics in IBD</v>
-      </c>
-      <c r="AL5" t="str">
-        <f t="shared" si="2"/>
-        <v>Antibiotics and Probiotics in IBD</v>
-      </c>
-      <c r="AM5" t="str">
-        <f>W5</f>
-        <v>What is IBD Remission: Adapting to a New Normal?</v>
-      </c>
-      <c r="AN5" t="str">
-        <f t="shared" si="0"/>
-        <v>Other or prefer not to say</v>
-      </c>
-      <c r="AO5" t="s">
-        <v>88</v>
-      </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>595286237</v>
       </c>
@@ -2169,27 +2012,8 @@
       <c r="AG6" t="s">
         <v>70</v>
       </c>
-      <c r="AK6" t="str">
-        <f t="shared" si="1"/>
-        <v>Low FODMAP Diet in IBD</v>
-      </c>
-      <c r="AL6" t="s">
-        <v>59</v>
-      </c>
-      <c r="AM6" t="str">
-        <f>X6</f>
-        <v>Travel with IBD</v>
-      </c>
-      <c r="AN6" t="str">
-        <f t="shared" si="0"/>
-        <v>Ulcerative colitis group</v>
-      </c>
-      <c r="AO6" t="str">
-        <f>AD6</f>
-        <v>Dating and Intimacy with IBD</v>
-      </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>595286237</v>
       </c>
@@ -2268,26 +2092,8 @@
       <c r="AG7" t="s">
         <v>77</v>
       </c>
-      <c r="AK7" t="s">
-        <v>101</v>
-      </c>
-      <c r="AL7" t="s">
-        <v>59</v>
-      </c>
-      <c r="AM7" t="str">
-        <f>X7</f>
-        <v>IBD Outside the Gut</v>
-      </c>
-      <c r="AN7" t="str">
-        <f t="shared" si="0"/>
-        <v>Family/Friend group</v>
-      </c>
-      <c r="AO7" t="str">
-        <f>W7</f>
-        <v>Dating and Intimacy with IBD</v>
-      </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>595352591</v>
       </c>
@@ -2384,28 +2190,8 @@
       <c r="AG8" t="s">
         <v>70</v>
       </c>
-      <c r="AK8" t="str">
-        <f>Z8</f>
-        <v>Antibiotics and Probiotics in IBD</v>
-      </c>
-      <c r="AL8" t="str">
-        <f t="shared" si="2"/>
-        <v>Parenting with IBD</v>
-      </c>
-      <c r="AM8" t="str">
-        <f>Y8</f>
-        <v>Microbiome in IBD</v>
-      </c>
-      <c r="AN8" t="str">
-        <f t="shared" si="0"/>
-        <v>Ulcerative colitis group</v>
-      </c>
-      <c r="AO8" t="str">
-        <f>W8</f>
-        <v>Exercising with IBD</v>
-      </c>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>595352591</v>
       </c>
@@ -2502,24 +2288,8 @@
       <c r="AG9" t="s">
         <v>70</v>
       </c>
-      <c r="AK9" t="str">
-        <f>Y9</f>
-        <v>Microbiome in IBD</v>
-      </c>
-      <c r="AL9" t="str">
-        <f>AB9</f>
-        <v>Emotional Health in IBD</v>
-      </c>
-      <c r="AN9" t="str">
-        <f t="shared" si="0"/>
-        <v>Ulcerative colitis group</v>
-      </c>
-      <c r="AO9" t="str">
-        <f>W9</f>
-        <v>Exercising with IBD</v>
-      </c>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>595442516</v>
       </c>
@@ -2616,20 +2386,8 @@
       <c r="AG10" t="s">
         <v>70</v>
       </c>
-      <c r="AK10" t="str">
-        <f t="shared" si="1"/>
-        <v>Emotional Health in IBD</v>
-      </c>
-      <c r="AL10" t="str">
-        <f t="shared" si="2"/>
-        <v>What is IBD Remission: Adapting to a New Normal?</v>
-      </c>
-      <c r="AN10" t="str">
-        <f t="shared" si="0"/>
-        <v>Ulcerative colitis group</v>
-      </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>595480414</v>
       </c>
@@ -2726,20 +2484,8 @@
       <c r="AG11" t="s">
         <v>77</v>
       </c>
-      <c r="AK11" t="str">
-        <f t="shared" si="1"/>
-        <v>Alternative therapies in IBD</v>
-      </c>
-      <c r="AL11" t="str">
-        <f t="shared" si="2"/>
-        <v>Low FODMAP Diet in IBD</v>
-      </c>
-      <c r="AN11" t="str">
-        <f t="shared" si="0"/>
-        <v>Family/Friend group</v>
-      </c>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>595480414</v>
       </c>
@@ -2836,20 +2582,8 @@
       <c r="AG12" t="s">
         <v>70</v>
       </c>
-      <c r="AK12" t="str">
-        <f t="shared" si="1"/>
-        <v>Alternative therapies in IBD</v>
-      </c>
-      <c r="AL12" t="str">
-        <f t="shared" si="2"/>
-        <v>Low FODMAP Diet in IBD</v>
-      </c>
-      <c r="AN12" t="str">
-        <f t="shared" si="0"/>
-        <v>Ulcerative colitis group</v>
-      </c>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>595500437</v>
       </c>
@@ -2946,20 +2680,8 @@
       <c r="AG13" t="s">
         <v>70</v>
       </c>
-      <c r="AK13" t="str">
-        <f t="shared" si="1"/>
-        <v>Flare Management and ADTU</v>
-      </c>
-      <c r="AL13" t="str">
-        <f t="shared" si="2"/>
-        <v>Antibiotics and Probiotics in IBD</v>
-      </c>
-      <c r="AN13" t="str">
-        <f t="shared" si="0"/>
-        <v>Ulcerative colitis group</v>
-      </c>
     </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>595574410</v>
       </c>
@@ -3056,20 +2778,8 @@
       <c r="AG14" t="s">
         <v>70</v>
       </c>
-      <c r="AK14" t="str">
-        <f t="shared" si="1"/>
-        <v>Low FODMAP Diet in IBD</v>
-      </c>
-      <c r="AL14" t="str">
-        <f t="shared" si="2"/>
-        <v>Microbiome in IBD</v>
-      </c>
-      <c r="AN14" t="str">
-        <f t="shared" si="0"/>
-        <v>Ulcerative colitis group</v>
-      </c>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>595574410</v>
       </c>
@@ -3166,20 +2876,8 @@
       <c r="AG15" t="s">
         <v>77</v>
       </c>
-      <c r="AK15" t="str">
-        <f t="shared" si="1"/>
-        <v>For Family Members: The Experience of Ulcerative Colitis</v>
-      </c>
-      <c r="AL15" t="str">
-        <f t="shared" si="2"/>
-        <v>Microbiome in IBD</v>
-      </c>
-      <c r="AN15" t="str">
-        <f t="shared" si="0"/>
-        <v>Family/Friend group</v>
-      </c>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>595671226</v>
       </c>
@@ -3276,20 +2974,8 @@
       <c r="AG16" t="s">
         <v>107</v>
       </c>
-      <c r="AK16" t="str">
-        <f t="shared" si="1"/>
-        <v>My Experience with IBD Surgery</v>
-      </c>
-      <c r="AL16" t="str">
-        <f t="shared" si="2"/>
-        <v>PTSD in IBD</v>
-      </c>
-      <c r="AN16" t="str">
-        <f t="shared" si="0"/>
-        <v>J pouch group</v>
-      </c>
     </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>595831267</v>
       </c>
@@ -3368,20 +3054,8 @@
       <c r="AG17" t="s">
         <v>70</v>
       </c>
-      <c r="AK17" t="str">
-        <f t="shared" si="1"/>
-        <v>Emotional Health in IBD</v>
-      </c>
-      <c r="AL17" t="str">
-        <f t="shared" si="2"/>
-        <v>Fatigue Reduction Diet</v>
-      </c>
-      <c r="AN17" t="str">
-        <f t="shared" si="0"/>
-        <v>Ulcerative colitis group</v>
-      </c>
     </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>596002939</v>
       </c>
@@ -3478,20 +3152,8 @@
       <c r="AG18" t="s">
         <v>70</v>
       </c>
-      <c r="AK18" t="str">
-        <f t="shared" si="1"/>
-        <v>Bone Loss in IBD</v>
-      </c>
-      <c r="AL18" t="str">
-        <f t="shared" si="2"/>
-        <v>Antibiotics and Probiotics in IBD</v>
-      </c>
-      <c r="AN18" t="str">
-        <f t="shared" si="0"/>
-        <v>Ulcerative colitis group</v>
-      </c>
     </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>596036984</v>
       </c>
@@ -3588,20 +3250,8 @@
       <c r="AG19" t="s">
         <v>117</v>
       </c>
-      <c r="AK19" t="str">
-        <f t="shared" si="1"/>
-        <v>Alternative therapies in IBD</v>
-      </c>
-      <c r="AL19" t="str">
-        <f t="shared" si="2"/>
-        <v>Emotional Health in IBD</v>
-      </c>
-      <c r="AN19" t="str">
-        <f t="shared" si="0"/>
-        <v>Crohn's Disease group</v>
-      </c>
     </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>596036984</v>
       </c>
@@ -3698,20 +3348,8 @@
       <c r="AG20" t="s">
         <v>117</v>
       </c>
-      <c r="AK20" t="str">
-        <f t="shared" si="1"/>
-        <v>For Family Members: The Experience of Crohn's Disease</v>
-      </c>
-      <c r="AL20" t="str">
-        <f t="shared" si="2"/>
-        <v>Alternative therapies in IBD</v>
-      </c>
-      <c r="AN20" t="str">
-        <f t="shared" si="0"/>
-        <v>Crohn's Disease group</v>
-      </c>
     </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>596038233</v>
       </c>
@@ -3790,20 +3428,8 @@
       <c r="AG21" t="s">
         <v>70</v>
       </c>
-      <c r="AK21" t="str">
-        <f t="shared" si="1"/>
-        <v>Low FODMAP Diet in IBD</v>
-      </c>
-      <c r="AL21" t="str">
-        <f t="shared" si="2"/>
-        <v>Fatigue Reduction Diet</v>
-      </c>
-      <c r="AN21" t="str">
-        <f t="shared" si="0"/>
-        <v>Ulcerative colitis group</v>
-      </c>
     </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>596264531</v>
       </c>
@@ -3900,20 +3526,8 @@
       <c r="AG22" t="s">
         <v>117</v>
       </c>
-      <c r="AK22" t="str">
-        <f t="shared" si="1"/>
-        <v>Transitions: Going to College &amp; Going to Work with IBD</v>
-      </c>
-      <c r="AL22" t="str">
-        <f t="shared" si="2"/>
-        <v>Acceptance in IBD &amp; Chronic Disease</v>
-      </c>
-      <c r="AN22" t="str">
-        <f t="shared" si="0"/>
-        <v>Crohn's Disease group</v>
-      </c>
     </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>596337714</v>
       </c>
@@ -4010,20 +3624,8 @@
       <c r="AG23" t="s">
         <v>70</v>
       </c>
-      <c r="AK23" t="str">
-        <f t="shared" si="1"/>
-        <v>Exercising with IBD</v>
-      </c>
-      <c r="AL23" t="str">
-        <f t="shared" si="2"/>
-        <v>Physical Therapy for Pain in IBD</v>
-      </c>
-      <c r="AN23" t="str">
-        <f t="shared" si="0"/>
-        <v>Ulcerative colitis group</v>
-      </c>
     </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>596450856</v>
       </c>
@@ -4120,20 +3722,8 @@
       <c r="AG24" t="s">
         <v>70</v>
       </c>
-      <c r="AK24" t="str">
-        <f t="shared" si="1"/>
-        <v>The Patient Perspective: Testing, Scoping, and Scanning in IBD</v>
-      </c>
-      <c r="AL24" t="str">
-        <f t="shared" si="2"/>
-        <v>PTSD in IBD</v>
-      </c>
-      <c r="AN24" t="str">
-        <f t="shared" si="0"/>
-        <v>Ulcerative colitis group</v>
-      </c>
     </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>596450856</v>
       </c>
@@ -4230,20 +3820,8 @@
       <c r="AG25" t="s">
         <v>77</v>
       </c>
-      <c r="AK25" t="str">
-        <f t="shared" si="1"/>
-        <v>The Patient Perspective: Testing, Scoping, and Scanning in IBD</v>
-      </c>
-      <c r="AL25" t="str">
-        <f t="shared" si="2"/>
-        <v>PTSD in IBD</v>
-      </c>
-      <c r="AN25" t="str">
-        <f t="shared" si="0"/>
-        <v>Family/Friend group</v>
-      </c>
     </row>
-    <row r="26" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>596573232</v>
       </c>
@@ -4322,20 +3900,8 @@
       <c r="AG26" t="s">
         <v>117</v>
       </c>
-      <c r="AK26" t="str">
-        <f t="shared" si="1"/>
-        <v>Emotional Health in IBD</v>
-      </c>
-      <c r="AL26" t="str">
-        <f t="shared" si="2"/>
-        <v>Fatigue Reduction Diet</v>
-      </c>
-      <c r="AN26" t="str">
-        <f t="shared" si="0"/>
-        <v>Crohn's Disease group</v>
-      </c>
     </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>595232847</v>
       </c>
@@ -4432,20 +3998,8 @@
       <c r="AG27" t="s">
         <v>70</v>
       </c>
-      <c r="AK27" t="str">
-        <f t="shared" si="1"/>
-        <v>What is IBD Remission: Adapting to a New Normal?</v>
-      </c>
-      <c r="AL27" t="str">
-        <f t="shared" si="2"/>
-        <v>Antibiotics and Probiotics in IBD</v>
-      </c>
-      <c r="AN27" t="str">
-        <f t="shared" si="0"/>
-        <v>Ulcerative colitis group</v>
-      </c>
     </row>
-    <row r="28" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>596633871</v>
       </c>
@@ -4542,20 +4096,8 @@
       <c r="AG28" t="s">
         <v>117</v>
       </c>
-      <c r="AK28" t="str">
-        <f t="shared" si="1"/>
-        <v>My Experience with IBD Surgery</v>
-      </c>
-      <c r="AL28" t="str">
-        <f t="shared" si="2"/>
-        <v>Insurance Challenges with IBD</v>
-      </c>
-      <c r="AN28" t="str">
-        <f t="shared" si="0"/>
-        <v>Crohn's Disease group</v>
-      </c>
     </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>596633871</v>
       </c>
@@ -4652,20 +4194,8 @@
       <c r="AG29" t="s">
         <v>117</v>
       </c>
-      <c r="AK29" t="str">
-        <f t="shared" si="1"/>
-        <v>My Experience with IBD Surgery</v>
-      </c>
-      <c r="AL29" t="str">
-        <f t="shared" si="2"/>
-        <v>Insurance Challenges with IBD</v>
-      </c>
-      <c r="AN29" t="str">
-        <f t="shared" si="0"/>
-        <v>Crohn's Disease group</v>
-      </c>
     </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>597548190</v>
       </c>
@@ -4744,20 +4274,8 @@
       <c r="AG30" t="s">
         <v>117</v>
       </c>
-      <c r="AK30" t="str">
-        <f t="shared" si="1"/>
-        <v>Emotional Health in IBD</v>
-      </c>
-      <c r="AL30" t="str">
-        <f t="shared" si="2"/>
-        <v>Exercising with IBD</v>
-      </c>
-      <c r="AN30" t="str">
-        <f t="shared" si="0"/>
-        <v>Crohn's Disease group</v>
-      </c>
     </row>
-    <row r="31" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>597554758</v>
       </c>
@@ -4836,20 +4354,8 @@
       <c r="AG31" t="s">
         <v>151</v>
       </c>
-      <c r="AK31" t="str">
-        <f t="shared" si="1"/>
-        <v>My Experience with IBD Surgery</v>
-      </c>
-      <c r="AL31" t="str">
-        <f t="shared" si="2"/>
-        <v>Exercising with IBD</v>
-      </c>
-      <c r="AN31" t="str">
-        <f t="shared" si="0"/>
-        <v>Other or prefer not to say</v>
-      </c>
     </row>
-    <row r="32" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>597587115</v>
       </c>
@@ -4946,20 +4452,8 @@
       <c r="AG32" t="s">
         <v>117</v>
       </c>
-      <c r="AK32" t="str">
-        <f t="shared" si="1"/>
-        <v>Dating and Intimacy with IBD</v>
-      </c>
-      <c r="AL32" t="str">
-        <f t="shared" si="2"/>
-        <v>Alternative therapies in IBD</v>
-      </c>
-      <c r="AN32" t="str">
-        <f t="shared" si="0"/>
-        <v>Crohn's Disease group</v>
-      </c>
     </row>
-    <row r="33" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>597869631</v>
       </c>
@@ -5056,20 +4550,8 @@
       <c r="AG33" t="s">
         <v>117</v>
       </c>
-      <c r="AK33" t="str">
-        <f t="shared" si="1"/>
-        <v>Living without Eating: The TPN Experience</v>
-      </c>
-      <c r="AL33" t="str">
-        <f t="shared" si="2"/>
-        <v>Bone Loss in IBD</v>
-      </c>
-      <c r="AN33" t="str">
-        <f t="shared" si="0"/>
-        <v>Crohn's Disease group</v>
-      </c>
     </row>
-    <row r="34" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>597869631</v>
       </c>
@@ -5166,20 +4648,8 @@
       <c r="AG34" t="s">
         <v>117</v>
       </c>
-      <c r="AK34" t="str">
-        <f t="shared" si="1"/>
-        <v>Living without Eating: The TPN Experience</v>
-      </c>
-      <c r="AL34" t="str">
-        <f t="shared" si="2"/>
-        <v>Bone Loss in IBD</v>
-      </c>
-      <c r="AN34" t="str">
-        <f t="shared" si="0"/>
-        <v>Crohn's Disease group</v>
-      </c>
     </row>
-    <row r="35" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>598000923</v>
       </c>
@@ -5258,20 +4728,8 @@
       <c r="AG35" t="s">
         <v>117</v>
       </c>
-      <c r="AK35" t="str">
-        <f t="shared" si="1"/>
-        <v>Microbiome in IBD</v>
-      </c>
-      <c r="AL35" t="str">
-        <f t="shared" si="2"/>
-        <v>Transitions: Going to College &amp; Going to Work with IBD</v>
-      </c>
-      <c r="AN35" t="str">
-        <f t="shared" si="0"/>
-        <v>Crohn's Disease group</v>
-      </c>
     </row>
-    <row r="36" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>598000923</v>
       </c>
@@ -5350,20 +4808,8 @@
       <c r="AG36" t="s">
         <v>117</v>
       </c>
-      <c r="AK36" t="str">
-        <f t="shared" si="1"/>
-        <v>Will My Baby Develop IBD?</v>
-      </c>
-      <c r="AL36" t="str">
-        <f t="shared" si="2"/>
-        <v>Will My Baby Develop IBD?</v>
-      </c>
-      <c r="AN36" t="str">
-        <f t="shared" si="0"/>
-        <v>Crohn's Disease group</v>
-      </c>
     </row>
-    <row r="37" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>598032143</v>
       </c>
@@ -5442,20 +4888,8 @@
       <c r="AG37" t="s">
         <v>151</v>
       </c>
-      <c r="AK37" t="str">
-        <f t="shared" si="1"/>
-        <v>Acceptance in IBD &amp; Chronic Disease</v>
-      </c>
-      <c r="AL37" t="str">
-        <f t="shared" si="2"/>
-        <v>Exercising with IBD</v>
-      </c>
-      <c r="AN37" t="str">
-        <f t="shared" si="0"/>
-        <v>Other or prefer not to say</v>
-      </c>
     </row>
-    <row r="38" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>598032143</v>
       </c>
@@ -5534,20 +4968,8 @@
       <c r="AG38" t="s">
         <v>151</v>
       </c>
-      <c r="AK38" t="str">
-        <f t="shared" si="1"/>
-        <v>What is IBD Remission: Adapting to a New Normal?</v>
-      </c>
-      <c r="AL38" t="str">
-        <f t="shared" si="2"/>
-        <v>Physical Therapy for Pain in IBD</v>
-      </c>
-      <c r="AN38" t="str">
-        <f t="shared" si="0"/>
-        <v>Other or prefer not to say</v>
-      </c>
     </row>
-    <row r="39" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>598041268</v>
       </c>
@@ -5626,20 +5048,8 @@
       <c r="AG39" t="s">
         <v>151</v>
       </c>
-      <c r="AK39" t="str">
-        <f t="shared" si="1"/>
-        <v>Exercising with IBD</v>
-      </c>
-      <c r="AL39" t="str">
-        <f t="shared" si="2"/>
-        <v>Antibiotics and Probiotics in IBD</v>
-      </c>
-      <c r="AN39" t="str">
-        <f t="shared" si="0"/>
-        <v>Other or prefer not to say</v>
-      </c>
     </row>
-    <row r="40" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>598041268</v>
       </c>
@@ -5718,20 +5128,8 @@
       <c r="AG40" t="s">
         <v>151</v>
       </c>
-      <c r="AK40" t="str">
-        <f t="shared" si="1"/>
-        <v>Alternative therapies in IBD</v>
-      </c>
-      <c r="AL40" t="str">
-        <f t="shared" si="2"/>
-        <v>PTSD in IBD</v>
-      </c>
-      <c r="AN40" t="str">
-        <f t="shared" si="0"/>
-        <v>Other or prefer not to say</v>
-      </c>
     </row>
-    <row r="41" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>598249770</v>
       </c>
@@ -5828,20 +5226,8 @@
       <c r="AG41" t="s">
         <v>117</v>
       </c>
-      <c r="AK41" t="str">
-        <f t="shared" si="1"/>
-        <v>Travel with IBD</v>
-      </c>
-      <c r="AL41" t="str">
-        <f t="shared" si="2"/>
-        <v>The Patient Perspective: Testing, Scoping, and Scanning in IBD</v>
-      </c>
-      <c r="AN41" t="str">
-        <f t="shared" si="0"/>
-        <v>Crohn's Disease group</v>
-      </c>
     </row>
-    <row r="42" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>598267156</v>
       </c>
@@ -5938,20 +5324,8 @@
       <c r="AG42" t="s">
         <v>117</v>
       </c>
-      <c r="AK42" t="str">
-        <f>W42</f>
-        <v>Transitions: Going to College &amp; Going to Work with IBD</v>
-      </c>
-      <c r="AL42" t="str">
-        <f t="shared" si="2"/>
-        <v>Exercising with IBD</v>
-      </c>
-      <c r="AN42" t="str">
-        <f t="shared" si="0"/>
-        <v>Crohn's Disease group</v>
-      </c>
     </row>
-    <row r="43" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>598267156</v>
       </c>
@@ -6048,20 +5422,8 @@
       <c r="AG43" t="s">
         <v>117</v>
       </c>
-      <c r="AK43" t="str">
-        <f t="shared" si="1"/>
-        <v>Transitions: Going to College &amp; Going to Work with IBD</v>
-      </c>
-      <c r="AL43" t="str">
-        <f t="shared" si="2"/>
-        <v>Exercising with IBD</v>
-      </c>
-      <c r="AN43" t="str">
-        <f t="shared" si="0"/>
-        <v>Crohn's Disease group</v>
-      </c>
     </row>
-    <row r="44" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>598296479</v>
       </c>
@@ -6158,20 +5520,8 @@
       <c r="AG44" t="s">
         <v>70</v>
       </c>
-      <c r="AK44" t="str">
-        <f t="shared" si="1"/>
-        <v>Microbiome in IBD</v>
-      </c>
-      <c r="AL44" t="str">
-        <f t="shared" si="2"/>
-        <v>Fatigue Reduction Diet</v>
-      </c>
-      <c r="AN44" t="str">
-        <f t="shared" si="0"/>
-        <v>Ulcerative colitis group</v>
-      </c>
     </row>
-    <row r="45" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>598363973</v>
       </c>
@@ -6268,20 +5618,8 @@
       <c r="AG45" t="s">
         <v>70</v>
       </c>
-      <c r="AK45" t="str">
-        <f t="shared" si="1"/>
-        <v>Transitions: Going to College &amp; Going to Work with IBD</v>
-      </c>
-      <c r="AL45" t="str">
-        <f t="shared" si="2"/>
-        <v>What is IBD Remission: Adapting to a New Normal?</v>
-      </c>
-      <c r="AN45" t="str">
-        <f t="shared" si="0"/>
-        <v>Ulcerative colitis group</v>
-      </c>
     </row>
-    <row r="46" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>598363973</v>
       </c>
@@ -6378,20 +5716,8 @@
       <c r="AG46" t="s">
         <v>77</v>
       </c>
-      <c r="AK46" t="str">
-        <f t="shared" si="1"/>
-        <v>Supporting a Partner or Family Member with IBD</v>
-      </c>
-      <c r="AL46" t="str">
-        <f t="shared" si="2"/>
-        <v>What is IBD Remission: Adapting to a New Normal?</v>
-      </c>
-      <c r="AN46" t="str">
-        <f t="shared" si="0"/>
-        <v>Family/Friend group</v>
-      </c>
     </row>
-    <row r="47" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>598774126</v>
       </c>
@@ -6488,20 +5814,8 @@
       <c r="AG47" t="s">
         <v>70</v>
       </c>
-      <c r="AK47" t="str">
-        <f t="shared" si="1"/>
-        <v>My Experience in Clinical Trials</v>
-      </c>
-      <c r="AL47" t="str">
-        <f t="shared" si="2"/>
-        <v>My Experience with A Stem Cell Clinical Trial for Fistulas in IBD</v>
-      </c>
-      <c r="AN47" t="str">
-        <f t="shared" si="0"/>
-        <v>Ulcerative colitis group</v>
-      </c>
     </row>
-    <row r="48" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>598774126</v>
       </c>
@@ -6598,20 +5912,8 @@
       <c r="AG48" t="s">
         <v>70</v>
       </c>
-      <c r="AK48" t="str">
-        <f t="shared" si="1"/>
-        <v>My Experience in Clinical Trials</v>
-      </c>
-      <c r="AL48" t="str">
-        <f t="shared" si="2"/>
-        <v>My Experience with A Stem Cell Clinical Trial for Fistulas in IBD</v>
-      </c>
-      <c r="AN48" t="str">
-        <f t="shared" si="0"/>
-        <v>Ulcerative colitis group</v>
-      </c>
     </row>
-    <row r="49" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>598774531</v>
       </c>
@@ -6708,20 +6010,8 @@
       <c r="AG49" t="s">
         <v>70</v>
       </c>
-      <c r="AK49" t="str">
-        <f t="shared" si="1"/>
-        <v>My Experience in Clinical Trials</v>
-      </c>
-      <c r="AL49" t="str">
-        <f t="shared" si="2"/>
-        <v>My Experience with A Stem Cell Clinical Trial for Fistulas in IBD</v>
-      </c>
-      <c r="AN49" t="str">
-        <f t="shared" si="0"/>
-        <v>Ulcerative colitis group</v>
-      </c>
     </row>
-    <row r="50" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>598774531</v>
       </c>
@@ -6818,20 +6108,8 @@
       <c r="AG50" t="s">
         <v>70</v>
       </c>
-      <c r="AK50" t="str">
-        <f t="shared" si="1"/>
-        <v>My Experience in Clinical Trials</v>
-      </c>
-      <c r="AL50" t="str">
-        <f t="shared" si="2"/>
-        <v>My Experience with A Stem Cell Clinical Trial for Fistulas in IBD</v>
-      </c>
-      <c r="AN50" t="str">
-        <f t="shared" si="0"/>
-        <v>Ulcerative colitis group</v>
-      </c>
     </row>
-    <row r="51" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>598778905</v>
       </c>
@@ -6910,20 +6188,8 @@
       <c r="AG51" t="s">
         <v>199</v>
       </c>
-      <c r="AK51" t="str">
-        <f t="shared" si="1"/>
-        <v>My Experience with A Stem Cell Clinical Trial for Fistulas in IBD</v>
-      </c>
-      <c r="AL51" t="str">
-        <f t="shared" si="2"/>
-        <v>Living with an Ostomy</v>
-      </c>
-      <c r="AN51" t="str">
-        <f t="shared" si="0"/>
-        <v>Ostomy group</v>
-      </c>
     </row>
-    <row r="52" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>598778905</v>
       </c>
@@ -7002,20 +6268,8 @@
       <c r="AG52" t="s">
         <v>77</v>
       </c>
-      <c r="AK52" t="str">
-        <f t="shared" si="1"/>
-        <v>My Experience with A Stem Cell Clinical Trial for Fistulas in IBD</v>
-      </c>
-      <c r="AL52" t="str">
-        <f t="shared" si="2"/>
-        <v>Supporting a Partner or Family Member with IBD</v>
-      </c>
-      <c r="AN52" t="str">
-        <f t="shared" si="0"/>
-        <v>Family/Friend group</v>
-      </c>
     </row>
-    <row r="53" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>598798128</v>
       </c>
@@ -7112,20 +6366,8 @@
       <c r="AG53" t="s">
         <v>151</v>
       </c>
-      <c r="AK53" t="str">
-        <f t="shared" si="1"/>
-        <v>Low FODMAP Diet in IBD</v>
-      </c>
-      <c r="AL53" t="str">
-        <f t="shared" si="2"/>
-        <v>Fatigue Reduction Diet</v>
-      </c>
-      <c r="AN53" t="str">
-        <f t="shared" si="0"/>
-        <v>Other or prefer not to say</v>
-      </c>
     </row>
-    <row r="54" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>598798128</v>
       </c>
@@ -7222,20 +6464,8 @@
       <c r="AG54" t="s">
         <v>151</v>
       </c>
-      <c r="AK54" t="str">
-        <f t="shared" si="1"/>
-        <v>Low FODMAP Diet in IBD</v>
-      </c>
-      <c r="AL54" t="str">
-        <f t="shared" si="2"/>
-        <v>Fatigue Reduction Diet</v>
-      </c>
-      <c r="AN54" t="str">
-        <f t="shared" si="0"/>
-        <v>Other or prefer not to say</v>
-      </c>
     </row>
-    <row r="55" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>598800662</v>
       </c>
@@ -7332,20 +6562,8 @@
       <c r="AG55" t="s">
         <v>117</v>
       </c>
-      <c r="AK55" t="str">
-        <f t="shared" si="1"/>
-        <v>Low FODMAP Diet in IBD</v>
-      </c>
-      <c r="AL55" t="str">
-        <f t="shared" si="2"/>
-        <v>Dating and Intimacy with IBD</v>
-      </c>
-      <c r="AN55" t="str">
-        <f t="shared" si="0"/>
-        <v>Crohn's Disease group</v>
-      </c>
     </row>
-    <row r="56" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>598800662</v>
       </c>
@@ -7442,20 +6660,8 @@
       <c r="AG56" t="s">
         <v>77</v>
       </c>
-      <c r="AK56" t="str">
-        <f t="shared" si="1"/>
-        <v>Low FODMAP Diet in IBD</v>
-      </c>
-      <c r="AL56" t="str">
-        <f t="shared" si="2"/>
-        <v>Dating and Intimacy with IBD</v>
-      </c>
-      <c r="AN56" t="str">
-        <f t="shared" si="0"/>
-        <v>Family/Friend group</v>
-      </c>
     </row>
-    <row r="57" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>598806142</v>
       </c>
@@ -7552,20 +6758,8 @@
       <c r="AG57" t="s">
         <v>77</v>
       </c>
-      <c r="AK57" t="str">
-        <f t="shared" si="1"/>
-        <v>For Family Members: The Experience of Crohn's Disease</v>
-      </c>
-      <c r="AL57" t="str">
-        <f t="shared" si="2"/>
-        <v>For Family Members: The Experience of Crohn's Disease</v>
-      </c>
-      <c r="AN57" t="str">
-        <f t="shared" si="0"/>
-        <v>Family/Friend group</v>
-      </c>
     </row>
-    <row r="58" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>598997289</v>
       </c>
@@ -7662,20 +6856,8 @@
       <c r="AG58" t="s">
         <v>70</v>
       </c>
-      <c r="AK58" t="str">
-        <f>W58</f>
-        <v>Antibiotics and Probiotics in IBD</v>
-      </c>
-      <c r="AL58" t="str">
-        <f t="shared" si="2"/>
-        <v>Bone Loss in IBD</v>
-      </c>
-      <c r="AN58" t="str">
-        <f t="shared" si="0"/>
-        <v>Ulcerative colitis group</v>
-      </c>
     </row>
-    <row r="59" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>598997289</v>
       </c>
@@ -7772,20 +6954,8 @@
       <c r="AG59" t="s">
         <v>70</v>
       </c>
-      <c r="AK59" t="str">
-        <f t="shared" si="1"/>
-        <v>Antibiotics and Probiotics in IBD</v>
-      </c>
-      <c r="AL59" t="str">
-        <f t="shared" si="2"/>
-        <v>Bone Loss in IBD</v>
-      </c>
-      <c r="AN59" t="str">
-        <f t="shared" si="0"/>
-        <v>Ulcerative colitis group</v>
-      </c>
     </row>
-    <row r="60" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>599180330</v>
       </c>
@@ -7882,20 +7052,8 @@
       <c r="AG60" t="s">
         <v>70</v>
       </c>
-      <c r="AK60" t="str">
-        <f t="shared" si="1"/>
-        <v>Emotional Health in IBD</v>
-      </c>
-      <c r="AL60" t="str">
-        <f t="shared" si="2"/>
-        <v>IBD Outside the Gut</v>
-      </c>
-      <c r="AN60" t="str">
-        <f t="shared" si="0"/>
-        <v>Ulcerative colitis group</v>
-      </c>
     </row>
-    <row r="61" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>599193011</v>
       </c>
@@ -7974,20 +7132,8 @@
       <c r="AG61" t="s">
         <v>117</v>
       </c>
-      <c r="AK61" t="str">
-        <f t="shared" si="1"/>
-        <v>Low FODMAP Diet in IBD</v>
-      </c>
-      <c r="AL61" t="str">
-        <f t="shared" si="2"/>
-        <v>Alternative therapies in IBD</v>
-      </c>
-      <c r="AN61" t="str">
-        <f t="shared" si="0"/>
-        <v>Crohn's Disease group</v>
-      </c>
     </row>
-    <row r="62" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>599193265</v>
       </c>
@@ -8084,20 +7230,8 @@
       <c r="AG62" t="s">
         <v>117</v>
       </c>
-      <c r="AK62" t="str">
-        <f t="shared" si="1"/>
-        <v>Antibiotics and Probiotics in IBD</v>
-      </c>
-      <c r="AL62" t="str">
-        <f t="shared" si="2"/>
-        <v>IBD Outside the Gut</v>
-      </c>
-      <c r="AN62" t="str">
-        <f t="shared" si="0"/>
-        <v>Crohn's Disease group</v>
-      </c>
     </row>
-    <row r="63" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>599193281</v>
       </c>
@@ -8194,20 +7328,8 @@
       <c r="AG63" t="s">
         <v>117</v>
       </c>
-      <c r="AK63" t="str">
-        <f t="shared" si="1"/>
-        <v>Transitions: Going to College &amp; Going to Work with IBD</v>
-      </c>
-      <c r="AL63" t="str">
-        <f t="shared" si="2"/>
-        <v>Antibiotics and Probiotics in IBD</v>
-      </c>
-      <c r="AN63" t="str">
-        <f t="shared" si="0"/>
-        <v>Crohn's Disease group</v>
-      </c>
     </row>
-    <row r="64" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>599643567</v>
       </c>
@@ -8304,20 +7426,8 @@
       <c r="AG64" t="s">
         <v>117</v>
       </c>
-      <c r="AK64" t="str">
-        <f t="shared" si="1"/>
-        <v>Living without Eating: The TPN Experience</v>
-      </c>
-      <c r="AL64" t="str">
-        <f t="shared" si="2"/>
-        <v>Supporting a Partner or Family Member with IBD</v>
-      </c>
-      <c r="AN64" t="str">
-        <f t="shared" si="0"/>
-        <v>Crohn's Disease group</v>
-      </c>
     </row>
-    <row r="65" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>599655943</v>
       </c>
@@ -8396,20 +7506,8 @@
       <c r="AG65" t="s">
         <v>70</v>
       </c>
-      <c r="AK65" t="str">
-        <f t="shared" si="1"/>
-        <v>Alternative therapies in IBD</v>
-      </c>
-      <c r="AL65" t="str">
-        <f t="shared" si="2"/>
-        <v>Living without Eating: The TPN Experience</v>
-      </c>
-      <c r="AN65" t="str">
-        <f t="shared" si="0"/>
-        <v>Ulcerative colitis group</v>
-      </c>
     </row>
-    <row r="66" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>599683020</v>
       </c>
@@ -8506,20 +7604,8 @@
       <c r="AG66" t="s">
         <v>77</v>
       </c>
-      <c r="AK66" t="str">
-        <f t="shared" si="1"/>
-        <v>Emotional Health in IBD</v>
-      </c>
-      <c r="AL66" t="str">
-        <f t="shared" si="2"/>
-        <v>Living without Eating: The TPN Experience</v>
-      </c>
-      <c r="AN66" t="str">
-        <f t="shared" si="0"/>
-        <v>Family/Friend group</v>
-      </c>
     </row>
-    <row r="67" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>599683020</v>
       </c>
@@ -8616,20 +7702,8 @@
       <c r="AG67" t="s">
         <v>70</v>
       </c>
-      <c r="AK67" t="str">
-        <f t="shared" ref="AK67:AK73" si="3">W67</f>
-        <v>Emotional Health in IBD</v>
-      </c>
-      <c r="AL67" t="str">
-        <f t="shared" ref="AL67:AL123" si="4">X67</f>
-        <v>Living without Eating: The TPN Experience</v>
-      </c>
-      <c r="AN67" t="str">
-        <f t="shared" ref="AN67:AN123" si="5">AG67</f>
-        <v>Ulcerative colitis group</v>
-      </c>
     </row>
-    <row r="68" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>599835648</v>
       </c>
@@ -8726,20 +7800,8 @@
       <c r="AG68" t="s">
         <v>107</v>
       </c>
-      <c r="AK68" t="str">
-        <f t="shared" si="3"/>
-        <v>Microbiome in IBD</v>
-      </c>
-      <c r="AL68" t="str">
-        <f t="shared" si="4"/>
-        <v>My Experience with A Stem Cell Clinical Trial for Fistulas in IBD</v>
-      </c>
-      <c r="AN68" t="str">
-        <f t="shared" si="5"/>
-        <v>J pouch group</v>
-      </c>
     </row>
-    <row r="69" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>599880558</v>
       </c>
@@ -8836,20 +7898,8 @@
       <c r="AG69" t="s">
         <v>117</v>
       </c>
-      <c r="AK69" t="str">
-        <f t="shared" si="3"/>
-        <v>Low FODMAP Diet in IBD</v>
-      </c>
-      <c r="AL69" t="str">
-        <f t="shared" si="4"/>
-        <v>Antibiotics and Probiotics in IBD</v>
-      </c>
-      <c r="AN69" t="str">
-        <f t="shared" si="5"/>
-        <v>Crohn's Disease group</v>
-      </c>
     </row>
-    <row r="70" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>599880558</v>
       </c>
@@ -8946,20 +7996,8 @@
       <c r="AG70" t="s">
         <v>77</v>
       </c>
-      <c r="AK70" t="str">
-        <f t="shared" si="3"/>
-        <v>Low FODMAP Diet in IBD</v>
-      </c>
-      <c r="AL70" t="str">
-        <f t="shared" si="4"/>
-        <v>Antibiotics and Probiotics in IBD</v>
-      </c>
-      <c r="AN70" t="str">
-        <f t="shared" si="5"/>
-        <v>Family/Friend group</v>
-      </c>
     </row>
-    <row r="71" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>599982304</v>
       </c>
@@ -9056,20 +8094,8 @@
       <c r="AG71" t="s">
         <v>117</v>
       </c>
-      <c r="AK71" t="str">
-        <f t="shared" si="3"/>
-        <v>Physical Therapy for Pain in IBD</v>
-      </c>
-      <c r="AL71" t="str">
-        <f t="shared" si="4"/>
-        <v>Exercising with IBD</v>
-      </c>
-      <c r="AN71" t="str">
-        <f t="shared" si="5"/>
-        <v>Crohn's Disease group</v>
-      </c>
     </row>
-    <row r="72" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>599992502</v>
       </c>
@@ -9166,20 +8192,8 @@
       <c r="AG72" t="s">
         <v>77</v>
       </c>
-      <c r="AK72" t="str">
-        <f t="shared" si="3"/>
-        <v>Transitions: Going to College &amp; Going to Work with IBD</v>
-      </c>
-      <c r="AL72" t="str">
-        <f t="shared" si="4"/>
-        <v>Emotional Health in IBD</v>
-      </c>
-      <c r="AN72" t="str">
-        <f t="shared" si="5"/>
-        <v>Family/Friend group</v>
-      </c>
     </row>
-    <row r="73" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>599999174</v>
       </c>
@@ -9258,20 +8272,8 @@
       <c r="AG73" t="s">
         <v>199</v>
       </c>
-      <c r="AK73" t="str">
-        <f t="shared" si="3"/>
-        <v>Living with an Ostomy</v>
-      </c>
-      <c r="AL73" t="str">
-        <f t="shared" si="4"/>
-        <v>Fatigue Reduction Diet</v>
-      </c>
-      <c r="AN73" t="str">
-        <f t="shared" si="5"/>
-        <v>Ostomy group</v>
-      </c>
     </row>
-    <row r="74" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>600685234</v>
       </c>
@@ -9368,20 +8370,8 @@
       <c r="AG74" t="s">
         <v>70</v>
       </c>
-      <c r="AK74" t="str">
-        <f>W74</f>
-        <v>The Patient Perspective: Testing, Scoping, and Scanning in IBD</v>
-      </c>
-      <c r="AL74" t="str">
-        <f t="shared" si="4"/>
-        <v>Parenting with IBD</v>
-      </c>
-      <c r="AN74" t="str">
-        <f t="shared" si="5"/>
-        <v>Ulcerative colitis group</v>
-      </c>
     </row>
-    <row r="75" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>600718045</v>
       </c>
@@ -9460,20 +8450,8 @@
       <c r="AG75" t="s">
         <v>70</v>
       </c>
-      <c r="AK75" t="str">
-        <f t="shared" ref="AK75:AK104" si="6">W75</f>
-        <v>What is IBD Remission: Adapting to a New Normal?</v>
-      </c>
-      <c r="AL75" t="str">
-        <f t="shared" si="4"/>
-        <v>Alternative therapies in IBD</v>
-      </c>
-      <c r="AN75" t="str">
-        <f t="shared" si="5"/>
-        <v>Ulcerative colitis group</v>
-      </c>
     </row>
-    <row r="76" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>600718045</v>
       </c>
@@ -9552,20 +8530,8 @@
       <c r="AG76" t="s">
         <v>70</v>
       </c>
-      <c r="AK76" t="str">
-        <f t="shared" si="6"/>
-        <v>What is IBD Remission: Adapting to a New Normal?</v>
-      </c>
-      <c r="AL76" t="str">
-        <f t="shared" si="4"/>
-        <v>Alternative therapies in IBD</v>
-      </c>
-      <c r="AN76" t="str">
-        <f t="shared" si="5"/>
-        <v>Ulcerative colitis group</v>
-      </c>
     </row>
-    <row r="77" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>601107478</v>
       </c>
@@ -9662,20 +8628,8 @@
       <c r="AG77" t="s">
         <v>70</v>
       </c>
-      <c r="AK77" t="str">
-        <f t="shared" si="6"/>
-        <v>Alternative therapies in IBD</v>
-      </c>
-      <c r="AL77" t="str">
-        <f t="shared" si="4"/>
-        <v>Flare Management and ADTU</v>
-      </c>
-      <c r="AN77" t="str">
-        <f t="shared" si="5"/>
-        <v>Ulcerative colitis group</v>
-      </c>
     </row>
-    <row r="78" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>601127473</v>
       </c>
@@ -9772,20 +8726,8 @@
       <c r="AG78" t="s">
         <v>70</v>
       </c>
-      <c r="AK78" t="str">
-        <f t="shared" si="6"/>
-        <v>Antibiotics and Probiotics in IBD</v>
-      </c>
-      <c r="AL78" t="str">
-        <f t="shared" si="4"/>
-        <v>Bone Loss in IBD</v>
-      </c>
-      <c r="AN78" t="str">
-        <f t="shared" si="5"/>
-        <v>Ulcerative colitis group</v>
-      </c>
     </row>
-    <row r="79" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>601297760</v>
       </c>
@@ -9864,20 +8806,8 @@
       <c r="AG79" t="s">
         <v>117</v>
       </c>
-      <c r="AK79" t="str">
-        <f t="shared" si="6"/>
-        <v>Transitioning from Pediatric to Adult Care</v>
-      </c>
-      <c r="AL79" t="str">
-        <f t="shared" si="4"/>
-        <v>The Patient Perspective: Testing, Scoping, and Scanning in IBD</v>
-      </c>
-      <c r="AN79" t="str">
-        <f t="shared" si="5"/>
-        <v>Crohn's Disease group</v>
-      </c>
     </row>
-    <row r="80" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>602357863</v>
       </c>
@@ -9956,20 +8886,8 @@
       <c r="AG80" t="s">
         <v>117</v>
       </c>
-      <c r="AK80" t="str">
-        <f t="shared" si="6"/>
-        <v>Flare Management and ADTU</v>
-      </c>
-      <c r="AL80" t="str">
-        <f t="shared" si="4"/>
-        <v>Alternative therapies in IBD</v>
-      </c>
-      <c r="AN80" t="str">
-        <f t="shared" si="5"/>
-        <v>Crohn's Disease group</v>
-      </c>
     </row>
-    <row r="81" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>602357863</v>
       </c>
@@ -10048,20 +8966,8 @@
       <c r="AG81" t="s">
         <v>77</v>
       </c>
-      <c r="AK81" t="str">
-        <f t="shared" si="6"/>
-        <v>Flare Management and ADTU</v>
-      </c>
-      <c r="AL81" t="str">
-        <f t="shared" si="4"/>
-        <v>Supporting a Partner or Family Member with IBD</v>
-      </c>
-      <c r="AN81" t="str">
-        <f t="shared" si="5"/>
-        <v>Family/Friend group</v>
-      </c>
     </row>
-    <row r="82" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>602991929</v>
       </c>
@@ -10158,20 +9064,8 @@
       <c r="AG82" t="s">
         <v>70</v>
       </c>
-      <c r="AK82" t="str">
-        <f t="shared" si="6"/>
-        <v>Microbiome in IBD</v>
-      </c>
-      <c r="AL82" t="str">
-        <f t="shared" si="4"/>
-        <v>Antibiotics and Probiotics in IBD</v>
-      </c>
-      <c r="AN82" t="str">
-        <f t="shared" si="5"/>
-        <v>Ulcerative colitis group</v>
-      </c>
     </row>
-    <row r="83" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>602991929</v>
       </c>
@@ -10268,20 +9162,8 @@
       <c r="AG83" t="s">
         <v>70</v>
       </c>
-      <c r="AK83" t="str">
-        <f t="shared" si="6"/>
-        <v>Microbiome in IBD</v>
-      </c>
-      <c r="AL83" t="str">
-        <f t="shared" si="4"/>
-        <v>Antibiotics and Probiotics in IBD</v>
-      </c>
-      <c r="AN83" t="str">
-        <f t="shared" si="5"/>
-        <v>Ulcerative colitis group</v>
-      </c>
     </row>
-    <row r="84" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>603003099</v>
       </c>
@@ -10378,20 +9260,8 @@
       <c r="AG84" t="s">
         <v>117</v>
       </c>
-      <c r="AK84" t="str">
-        <f t="shared" si="6"/>
-        <v>Microbiome in IBD</v>
-      </c>
-      <c r="AL84" t="str">
-        <f t="shared" si="4"/>
-        <v>Antibiotics and Probiotics in IBD</v>
-      </c>
-      <c r="AN84" t="str">
-        <f t="shared" si="5"/>
-        <v>Crohn's Disease group</v>
-      </c>
     </row>
-    <row r="85" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>603003099</v>
       </c>
@@ -10488,20 +9358,8 @@
       <c r="AG85" t="s">
         <v>117</v>
       </c>
-      <c r="AK85" t="str">
-        <f t="shared" si="6"/>
-        <v>Microbiome in IBD</v>
-      </c>
-      <c r="AL85" t="str">
-        <f t="shared" si="4"/>
-        <v>Antibiotics and Probiotics in IBD</v>
-      </c>
-      <c r="AN85" t="str">
-        <f t="shared" si="5"/>
-        <v>Crohn's Disease group</v>
-      </c>
     </row>
-    <row r="86" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>603214060</v>
       </c>
@@ -10580,20 +9438,8 @@
       <c r="AG86" t="s">
         <v>70</v>
       </c>
-      <c r="AK86" t="str">
-        <f t="shared" si="6"/>
-        <v>PTSD in IBD</v>
-      </c>
-      <c r="AL86" t="str">
-        <f t="shared" si="4"/>
-        <v>Living with an Ostomy</v>
-      </c>
-      <c r="AN86" t="str">
-        <f t="shared" si="5"/>
-        <v>Ulcerative colitis group</v>
-      </c>
     </row>
-    <row r="87" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>603214060</v>
       </c>
@@ -10672,20 +9518,8 @@
       <c r="AG87" t="s">
         <v>77</v>
       </c>
-      <c r="AK87" t="str">
-        <f t="shared" si="6"/>
-        <v>Physical Therapy for Pain in IBD</v>
-      </c>
-      <c r="AL87" t="str">
-        <f t="shared" si="4"/>
-        <v>Alternative therapies in IBD</v>
-      </c>
-      <c r="AN87" t="str">
-        <f t="shared" si="5"/>
-        <v>Family/Friend group</v>
-      </c>
     </row>
-    <row r="88" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>603318269</v>
       </c>
@@ -10782,20 +9616,8 @@
       <c r="AG88" t="s">
         <v>151</v>
       </c>
-      <c r="AK88" t="str">
-        <f t="shared" si="6"/>
-        <v>Microbiome in IBD</v>
-      </c>
-      <c r="AL88" t="str">
-        <f t="shared" si="4"/>
-        <v>IBD Outside the Gut</v>
-      </c>
-      <c r="AN88" t="str">
-        <f t="shared" si="5"/>
-        <v>Other or prefer not to say</v>
-      </c>
     </row>
-    <row r="89" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>603318269</v>
       </c>
@@ -10892,20 +9714,8 @@
       <c r="AG89" t="s">
         <v>151</v>
       </c>
-      <c r="AK89" t="str">
-        <f t="shared" si="6"/>
-        <v>Alternative therapies in IBD</v>
-      </c>
-      <c r="AL89" t="str">
-        <f t="shared" si="4"/>
-        <v>Exercising with IBD</v>
-      </c>
-      <c r="AN89" t="str">
-        <f t="shared" si="5"/>
-        <v>Other or prefer not to say</v>
-      </c>
     </row>
-    <row r="90" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>604150401</v>
       </c>
@@ -11002,20 +9812,8 @@
       <c r="AG90" t="s">
         <v>117</v>
       </c>
-      <c r="AK90" t="str">
-        <f t="shared" si="6"/>
-        <v>Fatigue Reduction Diet</v>
-      </c>
-      <c r="AL90" t="str">
-        <f t="shared" si="4"/>
-        <v>Low FODMAP Diet in IBD</v>
-      </c>
-      <c r="AN90" t="str">
-        <f t="shared" si="5"/>
-        <v>Crohn's Disease group</v>
-      </c>
     </row>
-    <row r="91" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>604150401</v>
       </c>
@@ -11112,20 +9910,8 @@
       <c r="AG91" t="s">
         <v>117</v>
       </c>
-      <c r="AK91" t="str">
-        <f t="shared" si="6"/>
-        <v>Fatigue Reduction Diet</v>
-      </c>
-      <c r="AL91" t="str">
-        <f t="shared" si="4"/>
-        <v>Low FODMAP Diet in IBD</v>
-      </c>
-      <c r="AN91" t="str">
-        <f t="shared" si="5"/>
-        <v>Crohn's Disease group</v>
-      </c>
     </row>
-    <row r="92" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>604611293</v>
       </c>
@@ -11222,20 +10008,8 @@
       <c r="AG92" t="s">
         <v>70</v>
       </c>
-      <c r="AK92" t="str">
-        <f t="shared" si="6"/>
-        <v>PTSD in IBD</v>
-      </c>
-      <c r="AL92" t="str">
-        <f t="shared" si="4"/>
-        <v>Flare Management and ADTU</v>
-      </c>
-      <c r="AN92" t="str">
-        <f t="shared" si="5"/>
-        <v>Ulcerative colitis group</v>
-      </c>
     </row>
-    <row r="93" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>605708883</v>
       </c>
@@ -11314,20 +10088,8 @@
       <c r="AG93" t="s">
         <v>151</v>
       </c>
-      <c r="AK93" t="str">
-        <f t="shared" si="6"/>
-        <v>Living without Eating: The TPN Experience</v>
-      </c>
-      <c r="AL93" t="str">
-        <f t="shared" si="4"/>
-        <v>Transitions: Going to College &amp; Going to Work with IBD</v>
-      </c>
-      <c r="AN93" t="str">
-        <f t="shared" si="5"/>
-        <v>Other or prefer not to say</v>
-      </c>
     </row>
-    <row r="94" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>606039968</v>
       </c>
@@ -11406,20 +10168,8 @@
       <c r="AG94" t="s">
         <v>117</v>
       </c>
-      <c r="AK94" t="str">
-        <f t="shared" si="6"/>
-        <v>Being Your Own Advocate in a Healthcare Setting</v>
-      </c>
-      <c r="AL94" t="str">
-        <f t="shared" si="4"/>
-        <v>Parenting with IBD</v>
-      </c>
-      <c r="AN94" t="str">
-        <f t="shared" si="5"/>
-        <v>Crohn's Disease group</v>
-      </c>
     </row>
-    <row r="95" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>606039968</v>
       </c>
@@ -11498,20 +10248,8 @@
       <c r="AG95" t="s">
         <v>77</v>
       </c>
-      <c r="AK95" t="str">
-        <f t="shared" si="6"/>
-        <v>For Family Members: The Experience of Crohn's Disease</v>
-      </c>
-      <c r="AL95" t="str">
-        <f t="shared" si="4"/>
-        <v>Supporting a Partner or Family Member with IBD</v>
-      </c>
-      <c r="AN95" t="str">
-        <f t="shared" si="5"/>
-        <v>Family/Friend group</v>
-      </c>
     </row>
-    <row r="96" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>606217907</v>
       </c>
@@ -11590,20 +10328,8 @@
       <c r="AG96" t="s">
         <v>117</v>
       </c>
-      <c r="AK96" t="str">
-        <f t="shared" si="6"/>
-        <v>My Experience with IBD Surgery</v>
-      </c>
-      <c r="AL96" t="str">
-        <f t="shared" si="4"/>
-        <v>The Patient Perspective: Testing, Scoping, and Scanning in IBD</v>
-      </c>
-      <c r="AN96" t="str">
-        <f t="shared" si="5"/>
-        <v>Crohn's Disease group</v>
-      </c>
     </row>
-    <row r="97" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>607410011</v>
       </c>
@@ -11700,20 +10426,8 @@
       <c r="AG97" t="s">
         <v>303</v>
       </c>
-      <c r="AK97" t="str">
-        <f t="shared" si="6"/>
-        <v>Managing School and 501 Plans with IBD (pediatric MD)</v>
-      </c>
-      <c r="AL97" t="str">
-        <f t="shared" si="4"/>
-        <v>Being Your Own Advocate in a Healthcare Setting</v>
-      </c>
-      <c r="AN97" t="str">
-        <f t="shared" si="5"/>
-        <v>Pediatric group</v>
-      </c>
     </row>
-    <row r="98" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>607614816</v>
       </c>
@@ -11810,20 +10524,8 @@
       <c r="AG98" t="s">
         <v>117</v>
       </c>
-      <c r="AK98" t="str">
-        <f t="shared" si="6"/>
-        <v>Microbiome in IBD</v>
-      </c>
-      <c r="AL98" t="str">
-        <f t="shared" si="4"/>
-        <v>Antibiotics and Probiotics in IBD</v>
-      </c>
-      <c r="AN98" t="str">
-        <f t="shared" si="5"/>
-        <v>Crohn's Disease group</v>
-      </c>
     </row>
-    <row r="99" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>607614816</v>
       </c>
@@ -11920,20 +10622,8 @@
       <c r="AG99" t="s">
         <v>117</v>
       </c>
-      <c r="AK99" t="str">
-        <f t="shared" si="6"/>
-        <v>Microbiome in IBD</v>
-      </c>
-      <c r="AL99" t="str">
-        <f t="shared" si="4"/>
-        <v>Antibiotics and Probiotics in IBD</v>
-      </c>
-      <c r="AN99" t="str">
-        <f t="shared" si="5"/>
-        <v>Crohn's Disease group</v>
-      </c>
     </row>
-    <row r="100" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>607792772</v>
       </c>
@@ -12012,20 +10702,8 @@
       <c r="AG100" t="s">
         <v>70</v>
       </c>
-      <c r="AK100" t="str">
-        <f t="shared" si="6"/>
-        <v>IBD Outside the Gut</v>
-      </c>
-      <c r="AL100" t="str">
-        <f t="shared" si="4"/>
-        <v>The Patient Perspective: Testing, Scoping, and Scanning in IBD</v>
-      </c>
-      <c r="AN100" t="str">
-        <f t="shared" si="5"/>
-        <v>Ulcerative colitis group</v>
-      </c>
     </row>
-    <row r="101" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>607792772</v>
       </c>
@@ -12104,20 +10782,8 @@
       <c r="AG101" t="s">
         <v>70</v>
       </c>
-      <c r="AK101" t="str">
-        <f t="shared" si="6"/>
-        <v>IBD Outside the Gut</v>
-      </c>
-      <c r="AL101" t="str">
-        <f t="shared" si="4"/>
-        <v>Antibiotics and Probiotics in IBD</v>
-      </c>
-      <c r="AN101" t="str">
-        <f t="shared" si="5"/>
-        <v>Ulcerative colitis group</v>
-      </c>
     </row>
-    <row r="102" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>607794160</v>
       </c>
@@ -12196,20 +10862,8 @@
       <c r="AG102" t="s">
         <v>70</v>
       </c>
-      <c r="AK102" t="str">
-        <f t="shared" si="6"/>
-        <v>IBD Outside the Gut</v>
-      </c>
-      <c r="AL102" t="str">
-        <f t="shared" si="4"/>
-        <v>The Patient Perspective: Testing, Scoping, and Scanning in IBD</v>
-      </c>
-      <c r="AN102" t="str">
-        <f t="shared" si="5"/>
-        <v>Ulcerative colitis group</v>
-      </c>
     </row>
-    <row r="103" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>608021787</v>
       </c>
@@ -12288,20 +10942,8 @@
       <c r="AG103" t="s">
         <v>117</v>
       </c>
-      <c r="AK103" t="str">
-        <f t="shared" si="6"/>
-        <v>Acceptance in IBD &amp; Chronic Disease</v>
-      </c>
-      <c r="AL103" t="str">
-        <f t="shared" si="4"/>
-        <v>PTSD in IBD</v>
-      </c>
-      <c r="AN103" t="str">
-        <f t="shared" si="5"/>
-        <v>Crohn's Disease group</v>
-      </c>
     </row>
-    <row r="104" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>608115991</v>
       </c>
@@ -12380,20 +11022,8 @@
       <c r="AG104" t="s">
         <v>117</v>
       </c>
-      <c r="AK104" t="str">
-        <f t="shared" si="6"/>
-        <v>Insurance Challenges with IBD</v>
-      </c>
-      <c r="AL104" t="str">
-        <f t="shared" si="4"/>
-        <v>PTSD in IBD</v>
-      </c>
-      <c r="AN104" t="str">
-        <f t="shared" si="5"/>
-        <v>Crohn's Disease group</v>
-      </c>
     </row>
-    <row r="105" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>608783288</v>
       </c>
@@ -12472,20 +11102,8 @@
       <c r="AG105" t="s">
         <v>117</v>
       </c>
-      <c r="AK105" t="str">
-        <f>W105</f>
-        <v>PTSD in IBD</v>
-      </c>
-      <c r="AL105" t="str">
-        <f t="shared" si="4"/>
-        <v>Fatigue Reduction Diet</v>
-      </c>
-      <c r="AN105" t="str">
-        <f t="shared" si="5"/>
-        <v>Crohn's Disease group</v>
-      </c>
     </row>
-    <row r="106" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>608898674</v>
       </c>
@@ -12582,20 +11200,8 @@
       <c r="AG106" t="s">
         <v>117</v>
       </c>
-      <c r="AK106" t="str">
-        <f t="shared" ref="AK106:AK123" si="7">W106</f>
-        <v>My Experience with A Stem Cell Clinical Trial for Fistulas in IBD</v>
-      </c>
-      <c r="AL106" t="str">
-        <f t="shared" si="4"/>
-        <v>Microbiome in IBD</v>
-      </c>
-      <c r="AN106" t="str">
-        <f t="shared" si="5"/>
-        <v>Crohn's Disease group</v>
-      </c>
     </row>
-    <row r="107" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>608898674</v>
       </c>
@@ -12692,20 +11298,8 @@
       <c r="AG107" t="s">
         <v>77</v>
       </c>
-      <c r="AK107" t="str">
-        <f t="shared" si="7"/>
-        <v>My Experience with A Stem Cell Clinical Trial for Fistulas in IBD</v>
-      </c>
-      <c r="AL107" t="str">
-        <f t="shared" si="4"/>
-        <v>Microbiome in IBD</v>
-      </c>
-      <c r="AN107" t="str">
-        <f t="shared" si="5"/>
-        <v>Family/Friend group</v>
-      </c>
     </row>
-    <row r="108" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>609130412</v>
       </c>
@@ -12802,20 +11396,8 @@
       <c r="AG108" t="s">
         <v>117</v>
       </c>
-      <c r="AK108" t="str">
-        <f t="shared" si="7"/>
-        <v>Alternative therapies in IBD</v>
-      </c>
-      <c r="AL108" t="str">
-        <f t="shared" si="4"/>
-        <v>My Experience with A Stem Cell Clinical Trial for Fistulas in IBD</v>
-      </c>
-      <c r="AN108" t="str">
-        <f t="shared" si="5"/>
-        <v>Crohn's Disease group</v>
-      </c>
     </row>
-    <row r="109" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>609142460</v>
       </c>
@@ -12894,20 +11476,8 @@
       <c r="AG109" t="s">
         <v>117</v>
       </c>
-      <c r="AK109" t="str">
-        <f t="shared" si="7"/>
-        <v>Transitions: Going to College &amp; Going to Work with IBD</v>
-      </c>
-      <c r="AL109" t="str">
-        <f t="shared" si="4"/>
-        <v>Supporting a Partner or Family Member with IBD</v>
-      </c>
-      <c r="AN109" t="str">
-        <f t="shared" si="5"/>
-        <v>Crohn's Disease group</v>
-      </c>
     </row>
-    <row r="110" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>609142460</v>
       </c>
@@ -12986,20 +11556,8 @@
       <c r="AG110" t="s">
         <v>77</v>
       </c>
-      <c r="AK110" t="str">
-        <f t="shared" si="7"/>
-        <v>For Family Members: The Experience of Crohn's Disease</v>
-      </c>
-      <c r="AL110" t="str">
-        <f t="shared" si="4"/>
-        <v>Transitions: Going to College &amp; Going to Work with IBD</v>
-      </c>
-      <c r="AN110" t="str">
-        <f t="shared" si="5"/>
-        <v>Family/Friend group</v>
-      </c>
     </row>
-    <row r="111" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>609268937</v>
       </c>
@@ -13096,20 +11654,8 @@
       <c r="AG111" t="s">
         <v>70</v>
       </c>
-      <c r="AK111" t="str">
-        <f t="shared" si="7"/>
-        <v>What is IBD Remission: Adapting to a New Normal?</v>
-      </c>
-      <c r="AL111" t="str">
-        <f t="shared" si="4"/>
-        <v>Parenting with IBD</v>
-      </c>
-      <c r="AN111" t="str">
-        <f t="shared" si="5"/>
-        <v>Ulcerative colitis group</v>
-      </c>
     </row>
-    <row r="112" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>609268937</v>
       </c>
@@ -13206,20 +11752,8 @@
       <c r="AG112" t="s">
         <v>77</v>
       </c>
-      <c r="AK112" t="str">
-        <f t="shared" si="7"/>
-        <v>For Family Members: The Experience of Ulcerative Colitis</v>
-      </c>
-      <c r="AL112" t="str">
-        <f t="shared" si="4"/>
-        <v>Supporting a Partner or Family Member with IBD</v>
-      </c>
-      <c r="AN112" t="str">
-        <f t="shared" si="5"/>
-        <v>Family/Friend group</v>
-      </c>
     </row>
-    <row r="113" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>609416981</v>
       </c>
@@ -13316,20 +11850,8 @@
       <c r="AG113" t="s">
         <v>117</v>
       </c>
-      <c r="AK113" t="str">
-        <f t="shared" si="7"/>
-        <v>Microbiome in IBD</v>
-      </c>
-      <c r="AL113" t="str">
-        <f t="shared" si="4"/>
-        <v>Antibiotics and Probiotics in IBD</v>
-      </c>
-      <c r="AN113" t="str">
-        <f t="shared" si="5"/>
-        <v>Crohn's Disease group</v>
-      </c>
     </row>
-    <row r="114" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>609484772</v>
       </c>
@@ -13426,20 +11948,8 @@
       <c r="AG114" t="s">
         <v>70</v>
       </c>
-      <c r="AK114" t="str">
-        <f t="shared" si="7"/>
-        <v>Antibiotics and Probiotics in IBD</v>
-      </c>
-      <c r="AL114" t="str">
-        <f t="shared" si="4"/>
-        <v>Exercising with IBD</v>
-      </c>
-      <c r="AN114" t="str">
-        <f t="shared" si="5"/>
-        <v>Ulcerative colitis group</v>
-      </c>
     </row>
-    <row r="115" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>609531115</v>
       </c>
@@ -13536,20 +12046,8 @@
       <c r="AG115" t="s">
         <v>117</v>
       </c>
-      <c r="AK115" t="str">
-        <f t="shared" si="7"/>
-        <v>Acceptance in IBD &amp; Chronic Disease</v>
-      </c>
-      <c r="AL115" t="str">
-        <f t="shared" si="4"/>
-        <v>Emotional Health in IBD</v>
-      </c>
-      <c r="AN115" t="str">
-        <f t="shared" si="5"/>
-        <v>Crohn's Disease group</v>
-      </c>
     </row>
-    <row r="116" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>609555061</v>
       </c>
@@ -13646,20 +12144,8 @@
       <c r="AG116" t="s">
         <v>70</v>
       </c>
-      <c r="AK116" t="str">
-        <f t="shared" si="7"/>
-        <v>Exercising with IBD</v>
-      </c>
-      <c r="AL116" t="str">
-        <f t="shared" si="4"/>
-        <v>Emotional Health in IBD</v>
-      </c>
-      <c r="AN116" t="str">
-        <f t="shared" si="5"/>
-        <v>Ulcerative colitis group</v>
-      </c>
     </row>
-    <row r="117" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>609555061</v>
       </c>
@@ -13756,20 +12242,8 @@
       <c r="AG117" t="s">
         <v>70</v>
       </c>
-      <c r="AK117" t="str">
-        <f t="shared" si="7"/>
-        <v>For Family Members: The Experience of Ulcerative Colitis</v>
-      </c>
-      <c r="AL117" t="str">
-        <f t="shared" si="4"/>
-        <v>Emotional Health in IBD</v>
-      </c>
-      <c r="AN117" t="str">
-        <f t="shared" si="5"/>
-        <v>Ulcerative colitis group</v>
-      </c>
     </row>
-    <row r="118" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>609844828</v>
       </c>
@@ -13848,20 +12322,8 @@
       <c r="AG118" t="s">
         <v>199</v>
       </c>
-      <c r="AK118" t="str">
-        <f t="shared" si="7"/>
-        <v>PTSD in IBD</v>
-      </c>
-      <c r="AL118" t="str">
-        <f t="shared" si="4"/>
-        <v>Being Your Own Advocate in a Healthcare Setting</v>
-      </c>
-      <c r="AN118" t="str">
-        <f t="shared" si="5"/>
-        <v>Ostomy group</v>
-      </c>
     </row>
-    <row r="119" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>609844828</v>
       </c>
@@ -13940,20 +12402,8 @@
       <c r="AG119" t="s">
         <v>199</v>
       </c>
-      <c r="AK119" t="str">
-        <f t="shared" si="7"/>
-        <v>The Patient Perspective: Testing, Scoping, and Scanning in IBD</v>
-      </c>
-      <c r="AL119" t="str">
-        <f t="shared" si="4"/>
-        <v>PTSD in IBD</v>
-      </c>
-      <c r="AN119" t="str">
-        <f t="shared" si="5"/>
-        <v>Ostomy group</v>
-      </c>
     </row>
-    <row r="120" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>609940459</v>
       </c>
@@ -14050,20 +12500,8 @@
       <c r="AG120" t="s">
         <v>77</v>
       </c>
-      <c r="AK120" t="str">
-        <f t="shared" si="7"/>
-        <v>Travel with IBD</v>
-      </c>
-      <c r="AL120" t="str">
-        <f t="shared" si="4"/>
-        <v>Travel with IBD</v>
-      </c>
-      <c r="AN120" t="str">
-        <f t="shared" si="5"/>
-        <v>Family/Friend group</v>
-      </c>
     </row>
-    <row r="121" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>609967069</v>
       </c>
@@ -14160,20 +12598,8 @@
       <c r="AG121" t="s">
         <v>117</v>
       </c>
-      <c r="AK121" t="str">
-        <f t="shared" si="7"/>
-        <v>Flare Management and ADTU</v>
-      </c>
-      <c r="AL121" t="str">
-        <f t="shared" si="4"/>
-        <v>Fatigue Reduction Diet</v>
-      </c>
-      <c r="AN121" t="str">
-        <f t="shared" si="5"/>
-        <v>Crohn's Disease group</v>
-      </c>
     </row>
-    <row r="122" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>609967069</v>
       </c>
@@ -14270,20 +12696,8 @@
       <c r="AG122" t="s">
         <v>117</v>
       </c>
-      <c r="AK122" t="str">
-        <f t="shared" si="7"/>
-        <v>Flare Management and ADTU</v>
-      </c>
-      <c r="AL122" t="str">
-        <f t="shared" si="4"/>
-        <v>Fatigue Reduction Diet</v>
-      </c>
-      <c r="AN122" t="str">
-        <f t="shared" si="5"/>
-        <v>Crohn's Disease group</v>
-      </c>
     </row>
-    <row r="123" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>610454420</v>
       </c>
@@ -14362,17 +12776,779 @@
       <c r="AG123" t="s">
         <v>77</v>
       </c>
-      <c r="AK123" t="str">
-        <f t="shared" si="7"/>
-        <v>For Family Members: The Experience of Crohn's Disease</v>
-      </c>
-      <c r="AL123" t="str">
-        <f t="shared" si="4"/>
-        <v>Antibiotics and Probiotics in IBD</v>
-      </c>
-      <c r="AN123" t="str">
-        <f t="shared" si="5"/>
-        <v>Family/Friend group</v>
+    </row>
+    <row r="124" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A124">
+        <v>610587042</v>
+      </c>
+      <c r="B124" s="1">
+        <v>42817.4220718</v>
+      </c>
+      <c r="C124" t="s">
+        <v>367</v>
+      </c>
+      <c r="D124" t="s">
+        <v>368</v>
+      </c>
+      <c r="E124" t="s">
+        <v>369</v>
+      </c>
+      <c r="F124">
+        <v>1</v>
+      </c>
+      <c r="G124" t="s">
+        <v>36</v>
+      </c>
+      <c r="H124">
+        <v>765731609</v>
+      </c>
+      <c r="J124" t="s">
+        <v>37</v>
+      </c>
+      <c r="K124" t="s">
+        <v>38</v>
+      </c>
+      <c r="L124">
+        <v>0</v>
+      </c>
+      <c r="M124">
+        <v>0</v>
+      </c>
+      <c r="N124">
+        <v>0</v>
+      </c>
+      <c r="O124">
+        <v>0</v>
+      </c>
+      <c r="P124" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q124" t="s">
+        <v>40</v>
+      </c>
+      <c r="R124" t="s">
+        <v>40</v>
+      </c>
+      <c r="S124" t="s">
+        <v>40</v>
+      </c>
+      <c r="T124" t="s">
+        <v>40</v>
+      </c>
+      <c r="U124" t="s">
+        <v>40</v>
+      </c>
+      <c r="V124" t="s">
+        <v>40</v>
+      </c>
+      <c r="W124" t="s">
+        <v>76</v>
+      </c>
+      <c r="X124" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y124" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z124" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA124" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB124" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC124" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD124" t="s">
+        <v>53</v>
+      </c>
+      <c r="AE124" t="s">
+        <v>72</v>
+      </c>
+      <c r="AF124" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG124" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="125" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A125">
+        <v>610621656</v>
+      </c>
+      <c r="B125" s="1">
+        <v>42817.473946799997</v>
+      </c>
+      <c r="C125" t="s">
+        <v>370</v>
+      </c>
+      <c r="D125" t="s">
+        <v>371</v>
+      </c>
+      <c r="E125" t="s">
+        <v>372</v>
+      </c>
+      <c r="F125">
+        <v>1</v>
+      </c>
+      <c r="G125" t="s">
+        <v>36</v>
+      </c>
+      <c r="H125">
+        <v>765773811</v>
+      </c>
+      <c r="J125" t="s">
+        <v>37</v>
+      </c>
+      <c r="K125" t="s">
+        <v>38</v>
+      </c>
+      <c r="L125">
+        <v>0</v>
+      </c>
+      <c r="M125">
+        <v>0</v>
+      </c>
+      <c r="N125">
+        <v>0</v>
+      </c>
+      <c r="O125">
+        <v>0</v>
+      </c>
+      <c r="P125" t="s">
+        <v>39</v>
+      </c>
+      <c r="W125" t="s">
+        <v>81</v>
+      </c>
+      <c r="X125" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y125" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z125" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA125" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB125" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC125" t="s">
+        <v>92</v>
+      </c>
+      <c r="AD125" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE125" t="s">
+        <v>66</v>
+      </c>
+      <c r="AF125" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG125" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="126" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A126">
+        <v>610648863</v>
+      </c>
+      <c r="B126" s="1">
+        <v>42817.512569400002</v>
+      </c>
+      <c r="C126" t="s">
+        <v>373</v>
+      </c>
+      <c r="D126" t="s">
+        <v>248</v>
+      </c>
+      <c r="E126" t="s">
+        <v>374</v>
+      </c>
+      <c r="F126">
+        <v>1</v>
+      </c>
+      <c r="G126" t="s">
+        <v>36</v>
+      </c>
+      <c r="H126">
+        <v>765806925</v>
+      </c>
+      <c r="J126" t="s">
+        <v>37</v>
+      </c>
+      <c r="K126" t="s">
+        <v>38</v>
+      </c>
+      <c r="L126">
+        <v>0</v>
+      </c>
+      <c r="M126">
+        <v>0</v>
+      </c>
+      <c r="N126">
+        <v>0</v>
+      </c>
+      <c r="O126">
+        <v>0</v>
+      </c>
+      <c r="P126" t="s">
+        <v>39</v>
+      </c>
+      <c r="W126" t="s">
+        <v>67</v>
+      </c>
+      <c r="X126" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y126" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z126" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA126" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB126" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC126" t="s">
+        <v>74</v>
+      </c>
+      <c r="AD126" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE126" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF126" t="s">
+        <v>72</v>
+      </c>
+      <c r="AG126" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="127" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A127">
+        <v>610655235</v>
+      </c>
+      <c r="B127" s="1">
+        <v>42817.521631900003</v>
+      </c>
+      <c r="C127" t="s">
+        <v>200</v>
+      </c>
+      <c r="D127" t="s">
+        <v>375</v>
+      </c>
+      <c r="E127" t="s">
+        <v>376</v>
+      </c>
+      <c r="F127">
+        <v>1</v>
+      </c>
+      <c r="G127" t="s">
+        <v>36</v>
+      </c>
+      <c r="H127">
+        <v>765814576</v>
+      </c>
+      <c r="J127" t="s">
+        <v>37</v>
+      </c>
+      <c r="K127" t="s">
+        <v>38</v>
+      </c>
+      <c r="L127">
+        <v>0</v>
+      </c>
+      <c r="M127">
+        <v>0</v>
+      </c>
+      <c r="N127">
+        <v>0</v>
+      </c>
+      <c r="O127">
+        <v>0</v>
+      </c>
+      <c r="P127" t="s">
+        <v>39</v>
+      </c>
+      <c r="W127" t="s">
+        <v>44</v>
+      </c>
+      <c r="X127" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y127" t="s">
+        <v>184</v>
+      </c>
+      <c r="Z127" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA127" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB127" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC127" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD127" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE127" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF127" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG127" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="128" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A128">
+        <v>610709227</v>
+      </c>
+      <c r="B128" s="1">
+        <v>42817.602951399997</v>
+      </c>
+      <c r="C128" t="s">
+        <v>377</v>
+      </c>
+      <c r="D128" t="s">
+        <v>378</v>
+      </c>
+      <c r="E128" t="s">
+        <v>379</v>
+      </c>
+      <c r="F128">
+        <v>1</v>
+      </c>
+      <c r="G128" t="s">
+        <v>36</v>
+      </c>
+      <c r="H128">
+        <v>765879504</v>
+      </c>
+      <c r="J128" t="s">
+        <v>37</v>
+      </c>
+      <c r="K128" t="s">
+        <v>38</v>
+      </c>
+      <c r="L128">
+        <v>0</v>
+      </c>
+      <c r="M128">
+        <v>0</v>
+      </c>
+      <c r="N128">
+        <v>0</v>
+      </c>
+      <c r="O128">
+        <v>0</v>
+      </c>
+      <c r="P128" t="s">
+        <v>39</v>
+      </c>
+      <c r="W128" t="s">
+        <v>57</v>
+      </c>
+      <c r="X128" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y128" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z128" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA128" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB128" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC128" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD128" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE128" t="s">
+        <v>106</v>
+      </c>
+      <c r="AF128" t="s">
+        <v>52</v>
+      </c>
+      <c r="AG128" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="129" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A129">
+        <v>610719641</v>
+      </c>
+      <c r="B129" s="1">
+        <v>42817.619513899997</v>
+      </c>
+      <c r="C129" t="s">
+        <v>380</v>
+      </c>
+      <c r="D129" t="s">
+        <v>381</v>
+      </c>
+      <c r="E129" t="s">
+        <v>382</v>
+      </c>
+      <c r="F129">
+        <v>1</v>
+      </c>
+      <c r="G129" t="s">
+        <v>36</v>
+      </c>
+      <c r="H129">
+        <v>765892248</v>
+      </c>
+      <c r="J129" t="s">
+        <v>37</v>
+      </c>
+      <c r="K129" t="s">
+        <v>38</v>
+      </c>
+      <c r="L129">
+        <v>0</v>
+      </c>
+      <c r="M129">
+        <v>0</v>
+      </c>
+      <c r="N129">
+        <v>0</v>
+      </c>
+      <c r="O129">
+        <v>0</v>
+      </c>
+      <c r="P129" t="s">
+        <v>39</v>
+      </c>
+      <c r="W129" t="s">
+        <v>81</v>
+      </c>
+      <c r="X129" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y129" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z129" t="s">
+        <v>83</v>
+      </c>
+      <c r="AA129" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB129" t="s">
+        <v>88</v>
+      </c>
+      <c r="AC129" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD129" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE129" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF129" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG129" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="130" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A130">
+        <v>610786036</v>
+      </c>
+      <c r="B130" s="1">
+        <v>42817.725312499999</v>
+      </c>
+      <c r="C130" t="s">
+        <v>218</v>
+      </c>
+      <c r="D130" t="s">
+        <v>383</v>
+      </c>
+      <c r="E130" t="s">
+        <v>384</v>
+      </c>
+      <c r="F130">
+        <v>1</v>
+      </c>
+      <c r="G130" t="s">
+        <v>36</v>
+      </c>
+      <c r="H130">
+        <v>765972555</v>
+      </c>
+      <c r="J130" t="s">
+        <v>37</v>
+      </c>
+      <c r="K130" t="s">
+        <v>38</v>
+      </c>
+      <c r="L130">
+        <v>0</v>
+      </c>
+      <c r="M130">
+        <v>0</v>
+      </c>
+      <c r="N130">
+        <v>0</v>
+      </c>
+      <c r="O130">
+        <v>0</v>
+      </c>
+      <c r="P130" t="s">
+        <v>39</v>
+      </c>
+      <c r="W130" t="s">
+        <v>67</v>
+      </c>
+      <c r="X130" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y130" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z130" t="s">
+        <v>81</v>
+      </c>
+      <c r="AA130" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB130" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC130" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD130" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE130" t="s">
+        <v>72</v>
+      </c>
+      <c r="AF130" t="s">
+        <v>74</v>
+      </c>
+      <c r="AG130" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="131" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A131">
+        <v>610788832</v>
+      </c>
+      <c r="B131" s="1">
+        <v>42817.730370400001</v>
+      </c>
+      <c r="C131" t="s">
+        <v>181</v>
+      </c>
+      <c r="D131" t="s">
+        <v>385</v>
+      </c>
+      <c r="E131" t="s">
+        <v>386</v>
+      </c>
+      <c r="F131">
+        <v>1</v>
+      </c>
+      <c r="G131" t="s">
+        <v>36</v>
+      </c>
+      <c r="H131">
+        <v>765975956</v>
+      </c>
+      <c r="J131" t="s">
+        <v>37</v>
+      </c>
+      <c r="K131" t="s">
+        <v>38</v>
+      </c>
+      <c r="L131">
+        <v>0</v>
+      </c>
+      <c r="M131">
+        <v>0</v>
+      </c>
+      <c r="N131">
+        <v>0</v>
+      </c>
+      <c r="O131">
+        <v>0</v>
+      </c>
+      <c r="P131" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q131" t="s">
+        <v>40</v>
+      </c>
+      <c r="R131" t="s">
+        <v>40</v>
+      </c>
+      <c r="S131" t="s">
+        <v>40</v>
+      </c>
+      <c r="T131" t="s">
+        <v>40</v>
+      </c>
+      <c r="U131" t="s">
+        <v>40</v>
+      </c>
+      <c r="V131" t="s">
+        <v>40</v>
+      </c>
+      <c r="W131" t="s">
+        <v>55</v>
+      </c>
+      <c r="X131" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y131" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z131" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA131" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB131" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC131" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD131" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE131" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF131" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG131" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="132" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A132">
+        <v>610820347</v>
+      </c>
+      <c r="B132" s="1">
+        <v>42817.792222199998</v>
+      </c>
+      <c r="C132" t="s">
+        <v>323</v>
+      </c>
+      <c r="D132" t="s">
+        <v>324</v>
+      </c>
+      <c r="E132" t="s">
+        <v>325</v>
+      </c>
+      <c r="F132">
+        <v>1</v>
+      </c>
+      <c r="G132" t="s">
+        <v>36</v>
+      </c>
+      <c r="H132">
+        <v>766014031</v>
+      </c>
+      <c r="J132" t="s">
+        <v>37</v>
+      </c>
+      <c r="K132" t="s">
+        <v>38</v>
+      </c>
+      <c r="L132">
+        <v>0</v>
+      </c>
+      <c r="M132">
+        <v>0</v>
+      </c>
+      <c r="N132">
+        <v>0</v>
+      </c>
+      <c r="O132">
+        <v>0</v>
+      </c>
+      <c r="P132" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q132" t="s">
+        <v>40</v>
+      </c>
+      <c r="R132" t="s">
+        <v>40</v>
+      </c>
+      <c r="S132" t="s">
+        <v>40</v>
+      </c>
+      <c r="T132" t="s">
+        <v>40</v>
+      </c>
+      <c r="U132" t="s">
+        <v>40</v>
+      </c>
+      <c r="V132" t="s">
+        <v>40</v>
+      </c>
+      <c r="W132" t="s">
+        <v>92</v>
+      </c>
+      <c r="X132" t="s">
+        <v>81</v>
+      </c>
+      <c r="Y132" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z132" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA132" t="s">
+        <v>184</v>
+      </c>
+      <c r="AB132" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC132" t="s">
+        <v>121</v>
+      </c>
+      <c r="AD132" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE132" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF132" t="s">
+        <v>106</v>
+      </c>
+      <c r="AG132" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>